<commit_message>
Add maven useful plugin info
</commit_message>
<xml_diff>
--- a/maven_lib.xlsx
+++ b/maven_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Language</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +66,65 @@
         -DartifactId=my-app 
         -DarchetypeArtifactId=maven-archetype-quickstart 
         -DinteractiveMode=false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maven</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jdk1.8 not compate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Build with dependency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>By default, Maven doesn't bundle dependencies in the JAR file it builds, and you're not providing them on the classpath when you're trying to execute your JAR file at the command-line. This is why the Java VM can't find the library class files when trying to execute your code.
+You could manually specify the libraries on the classpath with the -cp parameter, or There is a Maven plugin called the maven-shade-plugin to do this. You need to register it in your POM, and it will automatically build an "uber-JAR" containing your classes and the classes for your library code too when you run mvn package:
+  &lt;build&gt;
+    &lt;plugins&gt;
+      &lt;plugin&gt;
+        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
+        &lt;artifactId&gt;maven-shade-plugin&lt;/artifactId&gt;
+        &lt;version&gt;1.6&lt;/version&gt;
+        &lt;executions&gt;
+          &lt;execution&gt;
+            &lt;phase&gt;package&lt;/phase&gt;
+            &lt;goals&gt;
+              &lt;goal&gt;shade&lt;/goal&gt;
+            &lt;/goals&gt;
+          &lt;/execution&gt;
+        &lt;/executions&gt;
+      &lt;/plugin&gt;
+    &lt;/plugins&gt;
+  &lt;/build&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maven assumes to build witih jdk1.5, add below code to pom for other jdk version:
+  &lt;build&gt;
+    &lt;plugins&gt;
+   &lt;plugin&gt;
+        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
+        &lt;artifactId&gt;maven-compiler-plugin&lt;/artifactId&gt;
+        &lt;version&gt;3.3&lt;/version&gt;
+        &lt;configuration&gt;
+            &lt;source&gt;1.8&lt;/source&gt;
+            &lt;target&gt;1.8&lt;/target&gt;
+        &lt;/configuration&gt;
+   &lt;/plugin&gt;
+    &lt;/plugins&gt;
+  &lt;/build&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Build a jar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run "mvn package" under the target directory</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,20 +497,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="67.75" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="67.75" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -473,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -484,7 +543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -493,6 +552,39 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add autopay rest code
</commit_message>
<xml_diff>
--- a/maven_lib.xlsx
+++ b/maven_lib.xlsx
@@ -42,59 +42,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1. Generate necessary config file for eclipse:
-$mvn eclipse:eclipse -Dwtpversion=2.0
-2. Imports it into Eclipse IDE
-File -&gt; Import… -&gt; General -&gt; Existing Projects into workspace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>build a web project</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$ mvn archetype:generate 
-        -DgroupId={project-packaging} 
-        -DartifactId={project-name} 
-        -DarchetypeArtifactId=maven-archetype-webapp 
-        -DinteractiveMode=false</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$ mvn archetype:generate 
-        -DgroupId=com.mycompany.app
-        -DartifactId=my-app 
-        -DarchetypeArtifactId=maven-archetype-quickstart 
-        -DinteractiveMode=false</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Maven</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>jdk1.8 not compate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maven assumes to build witih jdk1.5, add below code to pom for other jdk version:
-  &lt;build&gt;
-    &lt;plugins&gt;
-   &lt;plugin&gt;
-        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
-        &lt;artifactId&gt;maven-compiler-plugin&lt;/artifactId&gt;
-        &lt;version&gt;3.3&lt;/version&gt;
-        &lt;configuration&gt;
-            &lt;source&gt;1.8&lt;/source&gt;
-            &lt;target&gt;1.8&lt;/target&gt;
-        &lt;/configuration&gt;
-   &lt;/plugin&gt;
-    &lt;/plugins&gt;
-  &lt;/build&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Build a jar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -178,6 +134,45 @@
     &lt;/build&gt;
 &lt;/project&gt;</t>
   </si>
+  <si>
+    <t>$ mvn archetype:generate 
+        -DgroupId=com.mycompany.app
+        -DartifactId=my-app 
+        -DarchetypeArtifactId=maven-archetype-quickstart 
+        -DinteractiveMode=false</t>
+  </si>
+  <si>
+    <t>1. Generate necessary config file for eclipse:
+$mvn eclipse:eclipse -Dwtpversion=2.0
+2. Imports it into Eclipse IDE
+File -&gt; Import… -&gt; General -&gt; Existing Projects into workspace</t>
+  </si>
+  <si>
+    <t>$ mvn archetype:generate 
+        -DgroupId={project-packaging} 
+        -DartifactId={project-name} 
+        -DarchetypeArtifactId=maven-archetype-webapp 
+        -DinteractiveMode=false</t>
+  </si>
+  <si>
+    <t>Maven assumes to build witih jdk1.5, add below code to pom for other jdk version:
+  &lt;build&gt;
+    &lt;plugins&gt;
+   &lt;plugin&gt;
+        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
+        &lt;artifactId&gt;maven-compiler-plugin&lt;/artifactId&gt;
+        &lt;version&gt;3.3&lt;/version&gt;
+        &lt;configuration&gt;
+            &lt;source&gt;1.8&lt;/source&gt;
+            &lt;target&gt;1.8&lt;/target&gt;
+        &lt;/configuration&gt;
+   &lt;/plugin&gt;
+    &lt;/plugins&gt;
+  &lt;/build&gt;</t>
+  </si>
+  <si>
+    <t>Build a jar</t>
+  </si>
 </sst>
 </file>
 
@@ -213,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,12 +240,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -549,7 +553,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="67.7109375" defaultRowHeight="36" customHeight="1"/>
@@ -574,11 +578,11 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="36" customHeight="1">
@@ -589,51 +593,51 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="36" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="36" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="36" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="36" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="36" customHeight="1">
@@ -641,10 +645,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add maven entry on udemy course notes
</commit_message>
<xml_diff>
--- a/maven_lib.xlsx
+++ b/maven_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,24 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
-  <si>
-    <t>Language</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Desc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Code Ref</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maven</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>build a java project</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -46,15 +34,127 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Maven</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jdk1.8 not compate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>run "mvn package" under the target directory</t>
+    <t>Build with dependency
+(maven-shade-plugin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build with dependency
+(maven-shade-plugin) 2 </t>
+  </si>
+  <si>
+    <t>Build a jar</t>
+  </si>
+  <si>
+    <t>build a project with interactive mode</t>
+  </si>
+  <si>
+    <t>Build a executable JAR</t>
+  </si>
+  <si>
+    <t>Build a window executable (*.exe)
+** not compete, need further work
+** use the launch4j plugin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;project xmlns="http://maven.apache.org/POM/4.0.0" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"
+  xsi:schemaLocation="http://maven.apache.org/POM/4.0.0 http://maven.apache.org/xsd/maven-4.0.0.xsd"&gt;
+  &lt;modelVersion&gt;4.0.0&lt;/modelVersion&gt;
+  &lt;groupId&gt;com.myles.util.ping&lt;/groupId&gt;
+  &lt;artifactId&gt;LocationTeller&lt;/artifactId&gt;
+  &lt;version&gt;1.0-SNAPSHOT&lt;/version&gt;
+  &lt;packaging&gt;jar&lt;/packaging&gt;
+  &lt;name&gt;LocationTeller&lt;/name&gt;
+  &lt;url&gt;http://maven.apache.org&lt;/url&gt;
+  &lt;properties&gt;
+    &lt;project.build.sourceEncoding&gt;UTF-8&lt;/project.build.sourceEncoding&gt;
+  &lt;/properties&gt;
+  &lt;dependencies&gt;
+    &lt;dependency&gt;
+      &lt;groupId&gt;junit&lt;/groupId&gt;
+      &lt;artifactId&gt;junit&lt;/artifactId&gt;
+      &lt;version&gt;3.8.1&lt;/version&gt;
+      &lt;scope&gt;test&lt;/scope&gt;
+    &lt;/dependency&gt;
+  &lt;/dependencies&gt;
+  &lt;build&gt;
+    &lt;plugins&gt;
+      &lt;plugin&gt;
+        &lt;artifactId&gt;maven-assembly-plugin&lt;/artifactId&gt;
+        &lt;configuration&gt;
+          &lt;archive&gt;
+            &lt;manifest&gt;
+              &lt;mainClass&gt;com.myles.util.ping.App&lt;/mainClass&gt;
+            &lt;/manifest&gt;
+          &lt;/archive&gt;
+          &lt;descriptorRefs&gt;
+            &lt;descriptorRef&gt;jar-with-dependencies&lt;/descriptorRef&gt;
+          &lt;/descriptorRefs&gt;
+        &lt;/configuration&gt;
+      &lt;/plugin&gt;
+    &lt;/plugins&gt;
+  &lt;/build&gt;
+&lt;/project&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># Mvn assume every "project" as "Artifact"
+# Lifecycle has diff phases:
+  - clean has 3 phases: pre-clean/clean/post-clean, and it uses the maven-clean-plugin with goal: clean
+  - site has 4 phases: pre-site/site/post-site/site-deploy
+  - default has 21 phases: (some common phases)
+    i) process-resource: copy resources to target
+ ii) compile
+ iii) test
+ iv) package: create jar/wars
+ v) install: to local repo
+ vi) deploy: to remote repo
+# If run the lifecycle n, mvn will auto run lifecycle 1.. n-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ mvn archetype:generate 
+        -DgroupId=com.mycompany.app
+        -DartifactId=my-app 
+        -DarchetypeArtifactId=maven-archetype-quickstart 
+        -DinteractiveMode=false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Generate necessary config file for eclipse:
+$mvn eclipse:eclipse -Dwtpversion=2.0
+2. Imports it into Eclipse IDE
+File -&gt; Import… -&gt; General -&gt; Existing Projects into workspace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ mvn archetype:generate 
+        -DgroupId={project-packaging} 
+        -DartifactId={project-name} 
+        -DarchetypeArtifactId=maven-archetype-webapp 
+        -DinteractiveMode=false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maven assumes to build witih jdk1.5, add below code to pom for other jdk version:
+  &lt;build&gt;
+    &lt;plugins&gt;
+   &lt;plugin&gt;
+        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
+        &lt;artifactId&gt;maven-compiler-plugin&lt;/artifactId&gt;
+        &lt;version&gt;3.3&lt;/version&gt;
+        &lt;configuration&gt;
+            &lt;source&gt;1.8&lt;/source&gt;
+            &lt;target&gt;1.8&lt;/target&gt;
+        &lt;/configuration&gt;
+   &lt;/plugin&gt;
+    &lt;/plugins&gt;
+  &lt;/build&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>By default, Maven doesn't bundle dependencies in the JAR file it builds, and you're not providing them on the classpath when you're trying to execute your JAR file at the command-line. This is why the Java VM can't find the library class files when trying to execute your code.
@@ -76,14 +176,11 @@
       &lt;/plugin&gt;
     &lt;/plugins&gt;
   &lt;/build&gt;</t>
-  </si>
-  <si>
-    <t>Build with dependency
-(maven-shade-plugin)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Build with dependency
-(maven-shade-plugin) 2 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run "mvn package" under the target directory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>According to spring.io, there is another parameter for shade plugin:
@@ -133,98 +230,11 @@
         &lt;/plugins&gt;
     &lt;/build&gt;
 &lt;/project&gt;</t>
-  </si>
-  <si>
-    <t>$ mvn archetype:generate 
-        -DgroupId=com.mycompany.app
-        -DartifactId=my-app 
-        -DarchetypeArtifactId=maven-archetype-quickstart 
-        -DinteractiveMode=false</t>
-  </si>
-  <si>
-    <t>1. Generate necessary config file for eclipse:
-$mvn eclipse:eclipse -Dwtpversion=2.0
-2. Imports it into Eclipse IDE
-File -&gt; Import… -&gt; General -&gt; Existing Projects into workspace</t>
-  </si>
-  <si>
-    <t>$ mvn archetype:generate 
-        -DgroupId={project-packaging} 
-        -DartifactId={project-name} 
-        -DarchetypeArtifactId=maven-archetype-webapp 
-        -DinteractiveMode=false</t>
-  </si>
-  <si>
-    <t>Maven assumes to build witih jdk1.5, add below code to pom for other jdk version:
-  &lt;build&gt;
-    &lt;plugins&gt;
-   &lt;plugin&gt;
-        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
-        &lt;artifactId&gt;maven-compiler-plugin&lt;/artifactId&gt;
-        &lt;version&gt;3.3&lt;/version&gt;
-        &lt;configuration&gt;
-            &lt;source&gt;1.8&lt;/source&gt;
-            &lt;target&gt;1.8&lt;/target&gt;
-        &lt;/configuration&gt;
-   &lt;/plugin&gt;
-    &lt;/plugins&gt;
-  &lt;/build&gt;</t>
-  </si>
-  <si>
-    <t>Build a jar</t>
-  </si>
-  <si>
-    <t>Maven</t>
-  </si>
-  <si>
-    <t>build a project with interactive mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>mvn archetype:generate</t>
-  </si>
-  <si>
-    <t>Build a executable JAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;project xmlns="http://maven.apache.org/POM/4.0.0" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"
-  xsi:schemaLocation="http://maven.apache.org/POM/4.0.0 http://maven.apache.org/xsd/maven-4.0.0.xsd"&gt;
-  &lt;modelVersion&gt;4.0.0&lt;/modelVersion&gt;
-  &lt;groupId&gt;com.myles.util.ping&lt;/groupId&gt;
-  &lt;artifactId&gt;LocationTeller&lt;/artifactId&gt;
-  &lt;version&gt;1.0-SNAPSHOT&lt;/version&gt;
-  &lt;packaging&gt;jar&lt;/packaging&gt;
-  &lt;name&gt;LocationTeller&lt;/name&gt;
-  &lt;url&gt;http://maven.apache.org&lt;/url&gt;
-  &lt;properties&gt;
-    &lt;project.build.sourceEncoding&gt;UTF-8&lt;/project.build.sourceEncoding&gt;
-  &lt;/properties&gt;
-  &lt;dependencies&gt;
-    &lt;dependency&gt;
-      &lt;groupId&gt;junit&lt;/groupId&gt;
-      &lt;artifactId&gt;junit&lt;/artifactId&gt;
-      &lt;version&gt;3.8.1&lt;/version&gt;
-      &lt;scope&gt;test&lt;/scope&gt;
-    &lt;/dependency&gt;
-  &lt;/dependencies&gt;
-  &lt;build&gt;
-    &lt;plugins&gt;
-      &lt;plugin&gt;
-        &lt;artifactId&gt;maven-assembly-plugin&lt;/artifactId&gt;
-        &lt;configuration&gt;
-          &lt;archive&gt;
-            &lt;manifest&gt;
-              &lt;mainClass&gt;com.myles.util.ping.App&lt;/mainClass&gt;
-            &lt;/manifest&gt;
-          &lt;/archive&gt;
-          &lt;descriptorRefs&gt;
-            &lt;descriptorRef&gt;jar-with-dependencies&lt;/descriptorRef&gt;
-          &lt;/descriptorRefs&gt;
-        &lt;/configuration&gt;
-      &lt;/plugin&gt;
-    &lt;/plugins&gt;
-  &lt;/build&gt;
-&lt;/project&gt;
-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">&lt;project xmlns="http://maven.apache.org/POM/4.0.0" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"
@@ -313,28 +323,89 @@
   &lt;/build&gt;
 &lt;/project&gt;
 </t>
-  </si>
-  <si>
-    <t>Build a window executable (*.exe)
-** not compete, need further work
-** use the launch4j plugin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code Ref</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maven</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maven</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Language</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># Likewise, plugins has different goals.
+# Maven is a plugin execution framework
+# The way to run maven plugin is like:
+ $ mvn maven-clean-plugin:clean
+ $ mvn maven-jar-plugin:jar
+ $ mvn archetype:generate
+# Different type of plugins: clean, compiler, surefile, jar, war, javadoc...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># central maven repo address: search.maven.org
+# local repo: default as .m2, and config setting.xml to change it.
+# remote repo is a custom repo specified in the pom.xml in the repositories tag.
+# search dependency seq: local&gt;central&gt;remote&gt;error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># module in a parent is useful to seperate packages but still remain the connection between different module in one big project
+# Parent mvn artifact pom.xml's pacakage is not jar but pom. And the module is some subfolder under parent directory using the module's artifact name.
+# Parent pom: son pom refers to parent pom
+# Aggregator pom: pom specify modules (And aggregator packaging turns into pom and it doesnt contain source by itself)
+# One more for aggregator mode, any mvn cmd run to aggregator, same mvn cmd auto apply to modules.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Udemy MooC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  -Lifecycle- clean
+  -Lifecycle- site
+  -Lifecycle- default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  -plugins
+  -plugins example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  -Maven repo </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  -Multiple modules
+  -Parent pom vs aggregator pom </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -342,14 +413,14 @@
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -399,7 +470,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -412,7 +483,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -486,6 +557,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -520,6 +592,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -695,140 +768,187 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="67.7109375" defaultRowHeight="36" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="67.75" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="36" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="36" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="36" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="36" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="36" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="36" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="36" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="137.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="36" customHeight="1">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="36" customHeight="1">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="36" customHeight="1">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
+    </row>
+    <row r="13" spans="1:3" ht="80.400000000000006" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="46.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -838,12 +958,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -851,12 +971,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add maven entry about install 3rd party jar to local repo
</commit_message>
<xml_diff>
--- a/maven_lib.xlsx
+++ b/maven_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Desc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -504,7 +504,7 @@
       <rPr>
         <sz val="8"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -515,7 +515,7 @@
       <rPr>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -543,22 +543,29 @@
     <t>Tag:build&gt; Tag:plugin (2)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Install 3rd party jars</t>
+  </si>
+  <si>
+    <t>mvn install:install-file -Dfile=&lt;path-to-file&gt; -DgroupId=&lt;group-id&gt; \
+    -DartifactId=&lt;artifact-id&gt; -Dversion=&lt;version&gt; -Dpackaging=&lt;packaging&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -566,21 +573,21 @@
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -631,7 +638,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -644,7 +651,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -718,7 +725,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -753,7 +759,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -929,21 +934,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="67.75" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="67.7109375" defaultRowHeight="36" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -954,7 +959,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="36" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -965,7 +970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="36" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -976,7 +981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="36" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -987,7 +992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="36" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -998,7 +1003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="36" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1009,7 +1014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="36" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1020,7 +1025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="36" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1031,7 +1036,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="36" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1042,7 +1047,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="36" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1053,7 +1058,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="36" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -1064,7 +1069,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="137.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="147">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -1075,7 +1080,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="80.400000000000006" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="79.5">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -1086,7 +1091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="46.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="45.75">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1097,7 +1102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="91.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="102">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1108,7 +1113,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="36" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
@@ -1119,7 +1124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="36" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="36" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1141,7 +1146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="36" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1152,7 +1157,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="36" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -1163,7 +1168,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="36" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -1174,7 +1179,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="87.6" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
@@ -1185,7 +1190,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="36" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
@@ -1194,6 +1199,17 @@
       </c>
       <c r="C23" s="2" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="36" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1204,12 +1220,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1217,12 +1233,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add maven config on window executable plugin Launch4j
</commit_message>
<xml_diff>
--- a/maven_lib.xlsx
+++ b/maven_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>Desc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -549,6 +549,103 @@
   <si>
     <t>mvn install:install-file -Dfile=&lt;path-to-file&gt; -DgroupId=&lt;group-id&gt; \
     -DartifactId=&lt;artifact-id&gt; -Dversion=&lt;version&gt; -Dpackaging=&lt;packaging&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build window executable </t>
+  </si>
+  <si>
+    <t>Build runnable jar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;plugin&gt;
+        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
+        &lt;artifactId&gt;maven-shade-plugin&lt;/artifactId&gt;
+        &lt;version&gt;1.6&lt;/version&gt;
+        &lt;executions&gt;
+          &lt;execution&gt;
+            &lt;phase&gt;package&lt;/phase&gt;
+            &lt;goals&gt;
+              &lt;goal&gt;shade&lt;/goal&gt;
+            &lt;/goals&gt;
+          &lt;/execution&gt;
+        &lt;/executions&gt;
+        &lt;!-- Set main class --&gt;
+        &lt;configuration&gt;
+            &lt;shadedArtifactAttached&gt;true&lt;/shadedArtifactAttached&gt;
+            &lt;shadedClassifierName&gt;shaded&lt;/shadedClassifierName&gt;
+            &lt;transformers&gt;
+                &lt;transformer implementation="org.apache.maven.plugins.shade.resource.ManifestResourceTransformer"&gt;
+                    &lt;mainClass&gt;com.bcm.util.bcmf.App&lt;/mainClass&gt;
+                &lt;/transformer&gt;
+            &lt;/transformers&gt;
+        &lt;/configuration&gt;
+      &lt;/plugin&gt;</t>
+  </si>
+  <si>
+    <t>*** setting might need a runnable jar prequisition ***
+      &lt;plugin&gt;
+        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
+        &lt;artifactId&gt;maven-shade-plugin&lt;/artifactId&gt;
+        &lt;version&gt;1.6&lt;/version&gt;
+        &lt;executions&gt;
+          &lt;execution&gt;
+            &lt;phase&gt;package&lt;/phase&gt;
+            &lt;goals&gt;
+              &lt;goal&gt;shade&lt;/goal&gt;
+            &lt;/goals&gt;
+          &lt;/execution&gt;
+        &lt;/executions&gt;
+        &lt;!-- Set main class --&gt;
+        &lt;configuration&gt;
+            &lt;shadedArtifactAttached&gt;true&lt;/shadedArtifactAttached&gt;
+            &lt;shadedClassifierName&gt;shaded&lt;/shadedClassifierName&gt;
+            &lt;transformers&gt;
+                &lt;transformer implementation="org.apache.maven.plugins.shade.resource.ManifestResourceTransformer"&gt;
+                    &lt;mainClass&gt;com.bcm.util.bcmf.App&lt;/mainClass&gt;
+                &lt;/transformer&gt;
+            &lt;/transformers&gt;
+        &lt;/configuration&gt;
+      &lt;/plugin&gt;
+      &lt;!-- build exe plugin--&gt;
+      &lt;plugin&gt;
+         &lt;groupId&gt;com.akathist.maven.plugins.launch4j&lt;/groupId&gt;
+         &lt;artifactId&gt;launch4j-maven-plugin&lt;/artifactId&gt;
+         &lt;version&gt;1.5.1&lt;/version&gt;
+         &lt;executions&gt;
+           &lt;execution&gt;
+             &lt;id&gt;l4j-clui&lt;/id&gt;
+             &lt;phase&gt;package&lt;/phase&gt;
+             &lt;goals&gt;
+                 &lt;goal&gt;launch4j&lt;/goal&gt;
+             &lt;/goals&gt;
+             &lt;configuration&gt;
+               &lt;headerType&gt;console&lt;/headerType&gt;
+               &lt;jar&gt;${project.build.directory}/${artifactId}-${version}-shaded.jar&lt;/jar&gt;
+               &lt;outfile&gt;${project.build.directory}/bcmf.exe&lt;/outfile&gt;
+               &lt;downloadUrl&gt;http://java.com/download&lt;/downloadUrl&gt;
+               &lt;classPath&gt;
+                   &lt;mainClass&gt;com.bcm.util.bcmf.App&lt;/mainClass&gt;
+               &lt;/classPath&gt;
+               &lt;jre&gt;
+                   &lt;minVersion&gt;1.6.0&lt;/minVersion&gt;
+                   &lt;jdkPreference&gt;preferJre&lt;/jdkPreference&gt;
+               &lt;/jre&gt;
+               &lt;versionInfo&gt;
+                   &lt;fileVersion&gt;1.0.0.0&lt;/fileVersion&gt;
+                   &lt;txtFileVersion&gt;${project.version}&lt;/txtFileVersion&gt;
+                   &lt;fileDescription&gt;${project.name}&lt;/fileDescription&gt;
+                   &lt;copyright&gt;bcm&lt;/copyright&gt;
+                   &lt;productVersion&gt;1.0.0.0&lt;/productVersion&gt;
+                   &lt;txtProductVersion&gt;1.0.0.0&lt;/txtProductVersion&gt;
+                   &lt;productName&gt;${project.name}&lt;/productName&gt;
+                   &lt;companyName&gt;bcm&lt;/companyName&gt;
+                   &lt;internalName&gt;bcmf&lt;/internalName&gt;
+                   &lt;originalFilename&gt;bcmf.exe&lt;/originalFilename&gt;
+               &lt;/versionInfo&gt;
+             &lt;/configuration&gt;
+           &lt;/execution&gt;
+         &lt;/executions&gt;
+      &lt;/plugin&gt;</t>
   </si>
 </sst>
 </file>
@@ -935,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="67.7109375" defaultRowHeight="36" customHeight="1"/>
@@ -1210,6 +1307,28 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="36" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="36" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add maven entry on how to override plugin's configration
</commit_message>
<xml_diff>
--- a/maven_lib.xlsx
+++ b/maven_lib.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Desc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -462,14 +462,52 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tag:build&gt; Tag:plugin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Tag:build&gt; Tag:plugin (2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Install 3rd party jars</t>
+  </si>
+  <si>
+    <t>mvn install:install-file -Dfile=&lt;path-to-file&gt; -DgroupId=&lt;group-id&gt; \
+    -DartifactId=&lt;artifact-id&gt; -Dversion=&lt;version&gt; -Dpackaging=&lt;packaging&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build window executable </t>
+  </si>
+  <si>
+    <t>Build runnable jar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;plugin&gt;
+        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
+        &lt;artifactId&gt;maven-shade-plugin&lt;/artifactId&gt;
+        &lt;version&gt;1.6&lt;/version&gt;
+        &lt;executions&gt;
+          &lt;execution&gt;
+            &lt;phase&gt;package&lt;/phase&gt;
+            &lt;goals&gt;
+              &lt;goal&gt;shade&lt;/goal&gt;
+            &lt;/goals&gt;
+          &lt;/execution&gt;
+        &lt;/executions&gt;
+        &lt;!-- Set main class --&gt;
+        &lt;configuration&gt;
+            &lt;shadedArtifactAttached&gt;true&lt;/shadedArtifactAttached&gt;
+            &lt;shadedClassifierName&gt;shaded&lt;/shadedClassifierName&gt;
+            &lt;transformers&gt;
+                &lt;transformer implementation="org.apache.maven.plugins.shade.resource.ManifestResourceTransformer"&gt;
+                    &lt;mainClass&gt;com.bcm.util.bcmf.App&lt;/mainClass&gt;
+                &lt;/transformer&gt;
+            &lt;/transformers&gt;
+        &lt;/configuration&gt;
+      &lt;/plugin&gt;</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">一直並非特別明白在Build Tag 中的Plugin Tag 有何作用, 以下幾用: 
-1. 因為Maven 默認己Bind 了Default Plugin 到各個Phase, 若要Override 這些設定(用別的Plugin 或是調整Configuration ) 是需要用到Plugin Tag的
-2. 雖然可以手動運行Plugin:goal, 但可放入Plugin Tag 中自動化, 如此例:
+1. 修改參數: 因為Maven 默認己Bind 了Default Plugin 到各個Phase, 若要Override 這些設定(用別的Plugin 或是調整Configuration ) 是需要用到Plugin Tag的
+2. 綁定運作: 雖然可以手動運行Plugin:goal, 但可放入Plugin Tag 中自動化, 如此例:
 &lt;plugin&gt;
    &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
    &lt;artifactId&gt;maven-antrun-plugin&lt;/artifactId&gt;
@@ -529,7 +567,9 @@
 [INFO] Final Memory: 4M/44M
 [INFO] ------------------------------------------------------------------</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tag:build&gt; Tag:plugin</t>
   </si>
   <si>
     <t>(續上例子) 
@@ -537,49 +577,6 @@
 * Each plugin can have multiple goals.
 * You can define phase from where plugin should starts its processing using its phase element. We've used clean phase.
 * You can configure tasks to be executed by binding them to goals of plugin. We've bound echo task with run goal of maven-antrun-plugin.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tag:build&gt; Tag:plugin (2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Install 3rd party jars</t>
-  </si>
-  <si>
-    <t>mvn install:install-file -Dfile=&lt;path-to-file&gt; -DgroupId=&lt;group-id&gt; \
-    -DartifactId=&lt;artifact-id&gt; -Dversion=&lt;version&gt; -Dpackaging=&lt;packaging&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Build window executable </t>
-  </si>
-  <si>
-    <t>Build runnable jar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      &lt;plugin&gt;
-        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
-        &lt;artifactId&gt;maven-shade-plugin&lt;/artifactId&gt;
-        &lt;version&gt;1.6&lt;/version&gt;
-        &lt;executions&gt;
-          &lt;execution&gt;
-            &lt;phase&gt;package&lt;/phase&gt;
-            &lt;goals&gt;
-              &lt;goal&gt;shade&lt;/goal&gt;
-            &lt;/goals&gt;
-          &lt;/execution&gt;
-        &lt;/executions&gt;
-        &lt;!-- Set main class --&gt;
-        &lt;configuration&gt;
-            &lt;shadedArtifactAttached&gt;true&lt;/shadedArtifactAttached&gt;
-            &lt;shadedClassifierName&gt;shaded&lt;/shadedClassifierName&gt;
-            &lt;transformers&gt;
-                &lt;transformer implementation="org.apache.maven.plugins.shade.resource.ManifestResourceTransformer"&gt;
-                    &lt;mainClass&gt;com.bcm.util.bcmf.App&lt;/mainClass&gt;
-                &lt;/transformer&gt;
-            &lt;/transformers&gt;
-        &lt;/configuration&gt;
-      &lt;/plugin&gt;</t>
   </si>
   <si>
     <t>*** setting might need a runnable jar prequisition ***
@@ -610,7 +607,7 @@
       &lt;plugin&gt;
          &lt;groupId&gt;com.akathist.maven.plugins.launch4j&lt;/groupId&gt;
          &lt;artifactId&gt;launch4j-maven-plugin&lt;/artifactId&gt;
-         &lt;version&gt;1.5.1&lt;/version&gt;
+         &lt;version&gt;1.7.2&lt;/version&gt;
          &lt;executions&gt;
            &lt;execution&gt;
              &lt;id&gt;l4j-clui&lt;/id&gt;
@@ -647,12 +644,62 @@
          &lt;/executions&gt;
       &lt;/plugin&gt;</t>
   </si>
+  <si>
+    <t>override pom property in command line</t>
+  </si>
+  <si>
+    <t>mvn xxxxx -Dxxx=xxx</t>
+  </si>
+  <si>
+    <t>override property of plugin javadoc</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Below snippet in pom define where to output javadoc in command `mvn javadoc:javadoc`. Be aware that this plugin wont be invoked automatically. It will </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ONLY </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>be invoke when user invoke the plugin and its goal.
+&lt;plugins&gt;
+…
+      &lt;!-- javadoc generation --&gt;
+      &lt;plugin&gt;
+        &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
+        &lt;artifactId&gt;maven-javadoc-plugin&lt;/artifactId&gt;
+        &lt;version&gt;3.0.0-M1&lt;/version&gt;
+        &lt;configuration&gt;
+            &lt;reportOutputDirectory&gt;
+                ${project.reporting.outputDirectory}/../..
+            &lt;/reportOutputDirectory&gt;
+        &lt;/configuration&gt;
+      &lt;/plugin&gt;
+...
+&lt;/plugins&gt;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,6 +734,14 @@
       <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1032,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="67.7109375" defaultRowHeight="36" customHeight="1"/>
@@ -1281,10 +1336,10 @@
         <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="36" customHeight="1">
@@ -1292,10 +1347,10 @@
         <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="36" customHeight="1">
@@ -1303,10 +1358,10 @@
         <v>34</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="36" customHeight="1">
@@ -1314,10 +1369,10 @@
         <v>34</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="36" customHeight="1">
@@ -1325,10 +1380,32 @@
         <v>34</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="36" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="36" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>